<commit_message>
Nomenclatura adecauda Encuesta Satisfaccion HTBP Mayo
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Encuestas de Satisfaccion/HTBP_EncuestaSatisfaccion-150527.xlsx
+++ b/qualtcom/Procesos/Encuestas de Satisfaccion/HTBP_EncuestaSatisfaccion-150527.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Procesos\Encuestas de Satisfaccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Procesos\Encuestas de Satisfaccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Encuesta de Satisfacción al Cliente</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>HTBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1671,7 +1674,7 @@
   <dimension ref="A1:BT99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2243,7 +2246,9 @@
         <v>5</v>
       </c>
       <c r="E10" s="100"/>
-      <c r="F10" s="112"/>
+      <c r="F10" s="112" t="s">
+        <v>66</v>
+      </c>
       <c r="G10" s="119"/>
       <c r="H10" s="119"/>
       <c r="I10" s="119"/>

</xml_diff>